<commit_message>
Export Into Excel: Correct Column Names #93
</commit_message>
<xml_diff>
--- a/Examples/TestScenario.xlsx
+++ b/Examples/TestScenario.xlsx
@@ -16,19 +16,19 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="22">
   <si>
-    <t xml:space="preserve"> StartTime</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Id</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Latitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Longitude</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Altitude</t>
+    <t xml:space="preserve"> Time</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> ID</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Lat</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Long</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Alt</t>
   </si>
   <si>
     <t xml:space="preserve"> Roll</t>
@@ -43,43 +43,43 @@
     <t xml:space="preserve"> RxTxType</t>
   </si>
   <si>
-    <t xml:space="preserve"> AntennaType</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Gain_dB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> CenterFrequency_Hz</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> Bandwith_Hz</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> SignalToNoiseRatio_dB</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> XPos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> YPos</t>
-  </si>
-  <si>
-    <t xml:space="preserve"> ZPos</t>
+    <t xml:space="preserve"> AntType</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Gain</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> CenterFreq</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BandWith</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> SNR</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> x</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> y</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> z</t>
   </si>
   <si>
     <t xml:space="preserve"> Remark</t>
   </si>
   <si>
+    <t>The quick brown fox jumps over a lazy dog.</t>
+  </si>
+  <si>
     <t>Vom Ödipuskomplex maßlos gequält, übt Wilfried zyklisches Jodeln.</t>
   </si>
   <si>
+    <t>Falsches Üben von Xylophonmusik quält jeden größeren Zwerg.</t>
+  </si>
+  <si>
     <t>Franz jagt im komplett verwahrlosten Taxi quer durch Bayern.</t>
-  </si>
-  <si>
-    <t>Falsches Üben von Xylophonmusik quält jeden größeren Zwerg.</t>
-  </si>
-  <si>
-    <t>The quick brown fox jumps over a lazy dog.</t>
   </si>
 </sst>
 </file>
@@ -454,7 +454,7 @@
     <col min="18" max="18" width="62.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:18" ht="116.25" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:18" ht="60" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -515,52 +515,52 @@
         <v>0</v>
       </c>
       <c r="B2" s="2">
-        <v>-221</v>
+        <v>-444</v>
       </c>
       <c r="C2" s="2">
-        <v>49.761353593987948</v>
+        <v>47.684197573978061</v>
       </c>
       <c r="D2" s="2">
-        <v>6.6578928208203019</v>
+        <v>9.3970467716033603</v>
       </c>
       <c r="E2" s="2">
-        <v>2893</v>
+        <v>7388</v>
       </c>
       <c r="F2" s="2">
-        <v>26</v>
+        <v>-10</v>
       </c>
       <c r="G2" s="2">
-        <v>-32</v>
+        <v>3</v>
       </c>
       <c r="H2" s="2">
-        <v>70</v>
+        <v>-56</v>
       </c>
       <c r="I2" s="2">
-        <v>1</v>
+        <v>200</v>
       </c>
       <c r="J2" s="2">
         <v>255</v>
       </c>
       <c r="K2" s="2">
-        <v>91</v>
+        <v>60</v>
       </c>
       <c r="L2" s="2">
-        <v>9600000</v>
+        <v>8500000</v>
       </c>
       <c r="M2" s="2">
-        <v>19000</v>
+        <v>11000</v>
       </c>
       <c r="N2" s="2">
-        <v>89</v>
+        <v>136</v>
       </c>
       <c r="O2" s="2">
-        <v>-17</v>
+        <v>59</v>
       </c>
       <c r="P2" s="2">
-        <v>66</v>
+        <v>32</v>
       </c>
       <c r="Q2" s="2">
-        <v>-15</v>
+        <v>9</v>
       </c>
       <c r="R2" s="3" t="s">
         <v>18</v>
@@ -571,52 +571,52 @@
         <v>0</v>
       </c>
       <c r="B3" s="2">
-        <v>-491</v>
+        <v>-740</v>
       </c>
       <c r="C3" s="2">
-        <v>49.753238372237902</v>
+        <v>47.695732678231174</v>
       </c>
       <c r="D3" s="2">
-        <v>6.6555594339714661</v>
+        <v>9.4297245355518928</v>
       </c>
       <c r="E3" s="2">
-        <v>11065</v>
+        <v>1394</v>
       </c>
       <c r="F3" s="2">
-        <v>-86</v>
+        <v>26</v>
       </c>
       <c r="G3" s="2">
-        <v>-68</v>
+        <v>-89</v>
       </c>
       <c r="H3" s="2">
-        <v>-79</v>
+        <v>-52</v>
       </c>
       <c r="I3" s="2">
         <v>2</v>
       </c>
       <c r="J3" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K3" s="2">
-        <v>84</v>
+        <v>71</v>
       </c>
       <c r="L3" s="2">
-        <v>9100000</v>
+        <v>8900000</v>
       </c>
       <c r="M3" s="2">
-        <v>18000</v>
+        <v>12000</v>
       </c>
       <c r="N3" s="2">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="O3" s="2">
-        <v>36</v>
+        <v>55</v>
       </c>
       <c r="P3" s="2">
-        <v>60</v>
+        <v>-20</v>
       </c>
       <c r="Q3" s="2">
-        <v>-8</v>
+        <v>-62</v>
       </c>
       <c r="R3" s="3" t="s">
         <v>19</v>
@@ -627,55 +627,55 @@
         <v>0</v>
       </c>
       <c r="B4" s="2">
-        <v>-866</v>
+        <v>306</v>
       </c>
       <c r="C4" s="2">
-        <v>49.748946852759801</v>
+        <v>47.681331740886108</v>
       </c>
       <c r="D4" s="2">
-        <v>6.6645235702185062</v>
+        <v>9.4206465625590674</v>
       </c>
       <c r="E4" s="2">
-        <v>5268</v>
+        <v>4347</v>
       </c>
       <c r="F4" s="2">
-        <v>44</v>
+        <v>-29</v>
       </c>
       <c r="G4" s="2">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="H4" s="2">
-        <v>-84</v>
+        <v>-5</v>
       </c>
       <c r="I4" s="2">
-        <v>255</v>
+        <v>101</v>
       </c>
       <c r="J4" s="2">
-        <v>0</v>
+        <v>2</v>
       </c>
       <c r="K4" s="2">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="L4" s="2">
-        <v>8900000</v>
+        <v>9800000</v>
       </c>
       <c r="M4" s="2">
         <v>16000</v>
       </c>
       <c r="N4" s="2">
-        <v>99</v>
+        <v>134</v>
       </c>
       <c r="O4" s="2">
-        <v>26</v>
+        <v>51</v>
       </c>
       <c r="P4" s="2">
-        <v>12</v>
+        <v>-21</v>
       </c>
       <c r="Q4" s="2">
-        <v>-28</v>
+        <v>40</v>
       </c>
       <c r="R4" s="3" t="s">
-        <v>18</v>
+        <v>20</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.25">
@@ -683,55 +683,55 @@
         <v>0</v>
       </c>
       <c r="B5" s="2">
-        <v>455</v>
+        <v>-183</v>
       </c>
       <c r="C5" s="2">
-        <v>49.773953630075674</v>
+        <v>47.681572705305427</v>
       </c>
       <c r="D5" s="2">
-        <v>6.6645221989391468</v>
+        <v>9.4165398955014066</v>
       </c>
       <c r="E5" s="2">
-        <v>6900</v>
+        <v>3334</v>
       </c>
       <c r="F5" s="2">
-        <v>10</v>
+        <v>-27</v>
       </c>
       <c r="G5" s="2">
-        <v>60</v>
+        <v>-72</v>
       </c>
       <c r="H5" s="2">
-        <v>16</v>
+        <v>-51</v>
       </c>
       <c r="I5" s="2">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="J5" s="2">
-        <v>0</v>
+        <v>3</v>
       </c>
       <c r="K5" s="2">
-        <v>90</v>
+        <v>40</v>
       </c>
       <c r="L5" s="2">
-        <v>9500000</v>
+        <v>10400000</v>
       </c>
       <c r="M5" s="2">
         <v>13000</v>
       </c>
       <c r="N5" s="2">
-        <v>79</v>
+        <v>126</v>
       </c>
       <c r="O5" s="2">
-        <v>58</v>
+        <v>-60</v>
       </c>
       <c r="P5" s="2">
-        <v>35</v>
+        <v>-63</v>
       </c>
       <c r="Q5" s="2">
-        <v>55</v>
+        <v>-10</v>
       </c>
       <c r="R5" s="3" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.25">
@@ -739,55 +739,55 @@
         <v>0</v>
       </c>
       <c r="B6" s="2">
-        <v>-356</v>
+        <v>-506</v>
       </c>
       <c r="C6" s="2">
-        <v>49.789229230053266</v>
+        <v>47.691367571696794</v>
       </c>
       <c r="D6" s="2">
-        <v>6.6354251542248406</v>
+        <v>9.4329133150378581</v>
       </c>
       <c r="E6" s="2">
-        <v>2104</v>
+        <v>11854</v>
       </c>
       <c r="F6" s="2">
-        <v>15</v>
+        <v>69</v>
       </c>
       <c r="G6" s="2">
-        <v>-41</v>
+        <v>30</v>
       </c>
       <c r="H6" s="2">
-        <v>11</v>
+        <v>-85</v>
       </c>
       <c r="I6" s="2">
-        <v>2</v>
+        <v>103</v>
       </c>
       <c r="J6" s="2">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="K6" s="2">
-        <v>118</v>
+        <v>115</v>
       </c>
       <c r="L6" s="2">
-        <v>9700000</v>
+        <v>8800000</v>
       </c>
       <c r="M6" s="2">
-        <v>12000</v>
+        <v>14000</v>
       </c>
       <c r="N6" s="2">
-        <v>41</v>
+        <v>85</v>
       </c>
       <c r="O6" s="2">
-        <v>-31</v>
+        <v>-58</v>
       </c>
       <c r="P6" s="2">
-        <v>-9</v>
+        <v>-32</v>
       </c>
       <c r="Q6" s="2">
-        <v>46</v>
+        <v>-40</v>
       </c>
       <c r="R6" s="3" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.25">
@@ -795,55 +795,55 @@
         <v>0</v>
       </c>
       <c r="B7" s="2">
-        <v>-958</v>
+        <v>-64</v>
       </c>
       <c r="C7" s="2">
-        <v>49.762306216678631</v>
+        <v>47.673540236618607</v>
       </c>
       <c r="D7" s="2">
-        <v>6.6378497835146959</v>
+        <v>9.4130118527567816</v>
       </c>
       <c r="E7" s="2">
-        <v>6400</v>
+        <v>3039</v>
       </c>
       <c r="F7" s="2">
-        <v>25</v>
+        <v>-30</v>
       </c>
       <c r="G7" s="2">
-        <v>63</v>
+        <v>13</v>
       </c>
       <c r="H7" s="2">
-        <v>72</v>
+        <v>-39</v>
       </c>
       <c r="I7" s="2">
-        <v>0</v>
+        <v>103</v>
       </c>
       <c r="J7" s="2">
-        <v>255</v>
+        <v>2</v>
       </c>
       <c r="K7" s="2">
-        <v>44</v>
+        <v>13</v>
       </c>
       <c r="L7" s="2">
-        <v>9400000</v>
+        <v>9900000</v>
       </c>
       <c r="M7" s="2">
         <v>10000</v>
       </c>
       <c r="N7" s="2">
-        <v>125</v>
+        <v>71</v>
       </c>
       <c r="O7" s="2">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="P7" s="2">
-        <v>-73</v>
+        <v>-35</v>
       </c>
       <c r="Q7" s="2">
-        <v>36</v>
+        <v>-49</v>
       </c>
       <c r="R7" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.25">
@@ -851,55 +851,55 @@
         <v>0</v>
       </c>
       <c r="B8" s="2">
-        <v>-285</v>
+        <v>198</v>
       </c>
       <c r="C8" s="2">
-        <v>49.780809625217039</v>
+        <v>47.713251513591139</v>
       </c>
       <c r="D8" s="2">
-        <v>6.6601051012521628</v>
+        <v>9.4311152235341602</v>
       </c>
       <c r="E8" s="2">
-        <v>5295</v>
+        <v>10963</v>
       </c>
       <c r="F8" s="2">
-        <v>80</v>
+        <v>-78</v>
       </c>
       <c r="G8" s="2">
-        <v>-80</v>
+        <v>26</v>
       </c>
       <c r="H8" s="2">
-        <v>-76</v>
+        <v>-44</v>
       </c>
       <c r="I8" s="2">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="J8" s="2">
-        <v>255</v>
+        <v>0</v>
       </c>
       <c r="K8" s="2">
-        <v>29</v>
+        <v>16</v>
       </c>
       <c r="L8" s="2">
-        <v>9200000</v>
+        <v>9300000</v>
       </c>
       <c r="M8" s="2">
-        <v>13000</v>
+        <v>18000</v>
       </c>
       <c r="N8" s="2">
-        <v>1</v>
+        <v>19</v>
       </c>
       <c r="O8" s="2">
-        <v>-34</v>
+        <v>42</v>
       </c>
       <c r="P8" s="2">
-        <v>-57</v>
+        <v>-65</v>
       </c>
       <c r="Q8" s="2">
-        <v>-71</v>
+        <v>54</v>
       </c>
       <c r="R8" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.25">
@@ -907,52 +907,52 @@
         <v>0</v>
       </c>
       <c r="B9" s="2">
-        <v>741</v>
+        <v>261</v>
       </c>
       <c r="C9" s="2">
-        <v>49.765352929588012</v>
+        <v>47.716840315494593</v>
       </c>
       <c r="D9" s="2">
-        <v>6.6357239654176041</v>
+        <v>9.4340819395363518</v>
       </c>
       <c r="E9" s="2">
-        <v>3657</v>
+        <v>5299</v>
       </c>
       <c r="F9" s="2">
-        <v>85</v>
+        <v>57</v>
       </c>
       <c r="G9" s="2">
-        <v>-27</v>
+        <v>65</v>
       </c>
       <c r="H9" s="2">
-        <v>79</v>
+        <v>7</v>
       </c>
       <c r="I9" s="2">
-        <v>2</v>
+        <v>102</v>
       </c>
       <c r="J9" s="2">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="K9" s="2">
-        <v>135</v>
+        <v>90</v>
       </c>
       <c r="L9" s="2">
-        <v>10300000</v>
+        <v>8900000</v>
       </c>
       <c r="M9" s="2">
-        <v>10000</v>
+        <v>19000</v>
       </c>
       <c r="N9" s="2">
-        <v>111</v>
+        <v>86</v>
       </c>
       <c r="O9" s="2">
-        <v>-4</v>
+        <v>36</v>
       </c>
       <c r="P9" s="2">
-        <v>11</v>
+        <v>18</v>
       </c>
       <c r="Q9" s="2">
-        <v>4</v>
+        <v>-1</v>
       </c>
       <c r="R9" s="3" t="s">
         <v>21</v>
@@ -963,55 +963,55 @@
         <v>0</v>
       </c>
       <c r="B10" s="2">
-        <v>868</v>
+        <v>26</v>
       </c>
       <c r="C10" s="2">
-        <v>49.782015442129136</v>
+        <v>47.68771994901946</v>
       </c>
       <c r="D10" s="2">
-        <v>6.6602832788138571</v>
+        <v>9.4059525086396896</v>
       </c>
       <c r="E10" s="2">
-        <v>443</v>
+        <v>5903</v>
       </c>
       <c r="F10" s="2">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="G10" s="2">
-        <v>-85</v>
+        <v>-21</v>
       </c>
       <c r="H10" s="2">
-        <v>-48</v>
+        <v>60</v>
       </c>
       <c r="I10" s="2">
-        <v>102</v>
+        <v>200</v>
       </c>
       <c r="J10" s="2">
-        <v>0</v>
+        <v>255</v>
       </c>
       <c r="K10" s="2">
-        <v>112</v>
+        <v>82</v>
       </c>
       <c r="L10" s="2">
         <v>8600000</v>
       </c>
       <c r="M10" s="2">
-        <v>11000</v>
+        <v>14000</v>
       </c>
       <c r="N10" s="2">
-        <v>104</v>
+        <v>52</v>
       </c>
       <c r="O10" s="2">
-        <v>17</v>
+        <v>33</v>
       </c>
       <c r="P10" s="2">
-        <v>2</v>
+        <v>-35</v>
       </c>
       <c r="Q10" s="2">
-        <v>48</v>
+        <v>30</v>
       </c>
       <c r="R10" s="3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.25">
@@ -1019,25 +1019,25 @@
         <v>0</v>
       </c>
       <c r="B11" s="2">
-        <v>895</v>
+        <v>-533</v>
       </c>
       <c r="C11" s="2">
-        <v>49.775836397334757</v>
+        <v>47.683094400362137</v>
       </c>
       <c r="D11" s="2">
-        <v>6.6314294210736309</v>
+        <v>9.3999438235127855</v>
       </c>
       <c r="E11" s="2">
-        <v>11428</v>
+        <v>4600</v>
       </c>
       <c r="F11" s="2">
-        <v>-17</v>
+        <v>18</v>
       </c>
       <c r="G11" s="2">
-        <v>-90</v>
+        <v>84</v>
       </c>
       <c r="H11" s="2">
-        <v>-42</v>
+        <v>13</v>
       </c>
       <c r="I11" s="2">
         <v>0</v>
@@ -1046,28 +1046,28 @@
         <v>255</v>
       </c>
       <c r="K11" s="2">
-        <v>66</v>
+        <v>2</v>
       </c>
       <c r="L11" s="2">
-        <v>10400000</v>
+        <v>9800000</v>
       </c>
       <c r="M11" s="2">
-        <v>13000</v>
+        <v>19000</v>
       </c>
       <c r="N11" s="2">
-        <v>11</v>
+        <v>71</v>
       </c>
       <c r="O11" s="2">
-        <v>4</v>
+        <v>-16</v>
       </c>
       <c r="P11" s="2">
-        <v>-20</v>
+        <v>-8</v>
       </c>
       <c r="Q11" s="2">
-        <v>4</v>
+        <v>-52</v>
       </c>
       <c r="R11" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
     </row>
   </sheetData>

</xml_diff>